<commit_message>
asset manager; input blocker; avatar
</commit_message>
<xml_diff>
--- a/GameDataConfigTool/excels/Avatar.xlsx
+++ b/GameDataConfigTool/excels/Avatar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\UnityProjects\SynthMind\GameDataConfigTool\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A547640E-435E-496B-ADB1-CD05D037D270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBB7D74-F0A9-4E26-876D-9BB5B1D3D032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="7500" windowWidth="17130" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14955" yWindow="6405" windowWidth="17130" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>id|int</t>
   </si>
@@ -33,20 +33,164 @@
     <t>asset|string</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
+    <t>Avatar01</t>
+  </si>
+  <si>
+    <t>Avatar02</t>
+  </si>
+  <si>
+    <t>Avatar03</t>
+  </si>
+  <si>
+    <t>Avatar04</t>
+  </si>
+  <si>
+    <t>Avatar05</t>
+  </si>
+  <si>
+    <t>Avatar06</t>
+  </si>
+  <si>
+    <t>Avatar07</t>
+  </si>
+  <si>
+    <t>Avatar08</t>
+  </si>
+  <si>
+    <t>Avatar09</t>
+  </si>
+  <si>
+    <t>Avatar10</t>
+  </si>
+  <si>
+    <t>Avatar11</t>
+  </si>
+  <si>
+    <t>Avatar12</t>
+  </si>
+  <si>
+    <t>Avatar13</t>
+  </si>
+  <si>
+    <t>Avatar14</t>
+  </si>
+  <si>
+    <t>Avatar15</t>
+  </si>
+  <si>
+    <t>Avatar16</t>
+  </si>
+  <si>
+    <t>Avatar17</t>
+  </si>
+  <si>
+    <t>Avatar18</t>
+  </si>
+  <si>
+    <t>Avatar19</t>
+  </si>
+  <si>
+    <t>Avatar20</t>
+  </si>
+  <si>
+    <t>Avatar21</t>
+  </si>
+  <si>
+    <t>Avatar22</t>
+  </si>
+  <si>
+    <t>Avatar23</t>
+  </si>
+  <si>
+    <t>Avatar24</t>
+  </si>
+  <si>
+    <t>Avatar25</t>
+  </si>
+  <si>
+    <t>Avatar26</t>
+  </si>
+  <si>
+    <t>Avatar27</t>
+  </si>
+  <si>
+    <t>Avatar28</t>
+  </si>
+  <si>
+    <t>Avatar29</t>
+  </si>
+  <si>
+    <t>Avatar30</t>
+  </si>
+  <si>
+    <t>Avatar31</t>
+  </si>
+  <si>
+    <t>Avatar32</t>
+  </si>
+  <si>
+    <t>Avatar33</t>
+  </si>
+  <si>
+    <t>Avatar34</t>
+  </si>
+  <si>
+    <t>Avatar35</t>
+  </si>
+  <si>
+    <t>Avatar36</t>
+  </si>
+  <si>
+    <t>Avatar37</t>
+  </si>
+  <si>
+    <t>Avatar38</t>
+  </si>
+  <si>
+    <t>Avatar39</t>
+  </si>
+  <si>
+    <t>Avatar40</t>
+  </si>
+  <si>
+    <t>Avatar41</t>
+  </si>
+  <si>
+    <t>Avatar42</t>
+  </si>
+  <si>
+    <t>Avatar43</t>
+  </si>
+  <si>
+    <t>Avatar44</t>
+  </si>
+  <si>
+    <t>Avatar45</t>
+  </si>
+  <si>
+    <t>Avatar46</t>
+  </si>
+  <si>
+    <t>Avatar47</t>
+  </si>
+  <si>
+    <t>Avatar48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,7 +534,376 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>